<commit_message>
Use additional where " Rownum < x" to ensure nondirect path read
</commit_message>
<xml_diff>
--- a/OracleBenchmarks.xlsx
+++ b/OracleBenchmarks.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pramm/Documents/Projekte/rammpeter.github/oracle_benchmarks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E185DD0-A782-8144-AEF1-9084588A6AA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C000E3-D03A-4245-B6BE-D36AF19FF5D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3160" yWindow="2260" windowWidth="28240" windowHeight="17240" activeTab="1" xr2:uid="{94BF2A6F-DF63-3D44-AC4F-74C7E5880432}"/>
+    <workbookView xWindow="3160" yWindow="2260" windowWidth="28240" windowHeight="17240" activeTab="2" xr2:uid="{94BF2A6F-DF63-3D44-AC4F-74C7E5880432}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Compression Table 2023-01" sheetId="2" r:id="rId2"/>
+    <sheet name="2023-01 Compr. Table Exadata" sheetId="2" r:id="rId2"/>
+    <sheet name="2023-05 Compr. Table Linux" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="34">
   <si>
     <t>Benchmark results for Oracle Database</t>
   </si>
@@ -130,6 +131,15 @@
   </si>
   <si>
     <t>Buffer gets total</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19.18 auf Exadata X6-2L High Capacity </t>
+  </si>
+  <si>
+    <t>19.3 auf Linux 6 CPU DB in Docker</t>
   </si>
 </sst>
 </file>
@@ -299,7 +309,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Compression Table 2023-01'!$A$13</c:f>
+              <c:f>'2023-01 Compr. Table Exadata'!$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -322,7 +332,7 @@
           </c:marker>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'Compression Table 2023-01'!$B$11:$Q$12</c:f>
+              <c:f>'2023-01 Compr. Table Exadata'!$B$14:$Q$15</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="16"/>
                 <c:lvl>
@@ -400,7 +410,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Compression Table 2023-01'!$B$13:$Q$13</c:f>
+              <c:f>'2023-01 Compr. Table Exadata'!$B$16:$Q$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -464,7 +474,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Compression Table 2023-01'!$A$14</c:f>
+              <c:f>'2023-01 Compr. Table Exadata'!$A$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -487,7 +497,7 @@
           </c:marker>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'Compression Table 2023-01'!$B$11:$Q$12</c:f>
+              <c:f>'2023-01 Compr. Table Exadata'!$B$14:$Q$15</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="16"/>
                 <c:lvl>
@@ -565,7 +575,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Compression Table 2023-01'!$B$14:$Q$14</c:f>
+              <c:f>'2023-01 Compr. Table Exadata'!$B$17:$Q$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -617,7 +627,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Compression Table 2023-01'!$A$15</c:f>
+              <c:f>'2023-01 Compr. Table Exadata'!$A$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -640,7 +650,7 @@
           </c:marker>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'Compression Table 2023-01'!$B$11:$Q$12</c:f>
+              <c:f>'2023-01 Compr. Table Exadata'!$B$14:$Q$15</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="16"/>
                 <c:lvl>
@@ -718,7 +728,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Compression Table 2023-01'!$B$15:$Q$15</c:f>
+              <c:f>'2023-01 Compr. Table Exadata'!$B$18:$Q$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -785,7 +795,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Compression Table 2023-01'!$A$16</c:f>
+              <c:f>'2023-01 Compr. Table Exadata'!$A$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -808,7 +818,7 @@
           </c:marker>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'Compression Table 2023-01'!$B$11:$Q$12</c:f>
+              <c:f>'2023-01 Compr. Table Exadata'!$B$14:$Q$15</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="16"/>
                 <c:lvl>
@@ -886,7 +896,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Compression Table 2023-01'!$B$16:$Q$16</c:f>
+              <c:f>'2023-01 Compr. Table Exadata'!$B$19:$Q$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -953,7 +963,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Compression Table 2023-01'!$A$17</c:f>
+              <c:f>'2023-01 Compr. Table Exadata'!$A$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -976,7 +986,7 @@
           </c:marker>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'Compression Table 2023-01'!$B$11:$Q$12</c:f>
+              <c:f>'2023-01 Compr. Table Exadata'!$B$14:$Q$15</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="16"/>
                 <c:lvl>
@@ -1054,7 +1064,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Compression Table 2023-01'!$B$17:$Q$17</c:f>
+              <c:f>'2023-01 Compr. Table Exadata'!$B$20:$Q$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1121,7 +1131,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Compression Table 2023-01'!$A$18</c:f>
+              <c:f>'2023-01 Compr. Table Exadata'!$A$21</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1144,7 +1154,7 @@
           </c:marker>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'Compression Table 2023-01'!$B$11:$Q$12</c:f>
+              <c:f>'2023-01 Compr. Table Exadata'!$B$14:$Q$15</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="16"/>
                 <c:lvl>
@@ -1222,7 +1232,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Compression Table 2023-01'!$B$18:$Q$18</c:f>
+              <c:f>'2023-01 Compr. Table Exadata'!$B$21:$Q$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1289,7 +1299,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Compression Table 2023-01'!$A$19</c:f>
+              <c:f>'2023-01 Compr. Table Exadata'!$A$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1314,7 +1324,7 @@
           </c:marker>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'Compression Table 2023-01'!$B$11:$Q$12</c:f>
+              <c:f>'2023-01 Compr. Table Exadata'!$B$14:$Q$15</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="16"/>
                 <c:lvl>
@@ -1392,7 +1402,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Compression Table 2023-01'!$B$19:$Q$19</c:f>
+              <c:f>'2023-01 Compr. Table Exadata'!$B$22:$Q$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2218,13 +2228,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1435100</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>158750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2570,10 +2580,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CC0EE75-4D97-7149-ABEE-2D40575DB096}">
-  <dimension ref="A1:Q19"/>
+  <dimension ref="A2:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2588,505 +2598,805 @@
     <col min="16" max="16" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>14</v>
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>15</v>
+      <c r="A6" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
+    <row r="13" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
     </row>
-    <row r="11" spans="1:17" s="1" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+    <row r="14" spans="1:17" s="1" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B14" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C14" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D14" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8" t="s">
+      <c r="E14" s="8"/>
+      <c r="F14" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="8"/>
-      <c r="H11" s="9" t="s">
+      <c r="G14" s="8"/>
+      <c r="H14" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9" t="s">
+      <c r="I14" s="9"/>
+      <c r="J14" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9" t="s">
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9" t="s">
+      <c r="N14" s="9"/>
+      <c r="O14" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="P11" s="9"/>
-      <c r="Q11" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
     </row>
-    <row r="12" spans="1:17" s="3" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="10" t="s">
+    <row r="15" spans="1:17" s="3" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E15" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F15" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="12" t="s">
+      <c r="G15" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H15" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I12" s="12" t="s">
+      <c r="I15" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="J12" s="10" t="s">
+      <c r="J15" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K12" s="10" t="s">
+      <c r="K15" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="L12" s="12" t="s">
+      <c r="L15" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="M12" s="10" t="s">
+      <c r="M15" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="N12" s="12" t="s">
+      <c r="N15" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="O12" s="10" t="s">
+      <c r="O15" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="P12" s="10" t="s">
+      <c r="P15" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="Q12" s="12" t="s">
+      <c r="Q15" s="12" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="14">
-        <v>2638</v>
-      </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="15">
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="E13" s="14">
-        <v>1</v>
-      </c>
-      <c r="F13" s="15">
-        <v>17.033000000000001</v>
-      </c>
-      <c r="G13" s="16">
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="H13" s="14">
-        <v>0.76400000000000001</v>
-      </c>
-      <c r="I13" s="14">
-        <v>4.9700000000000001E-2</v>
-      </c>
-      <c r="J13" s="15">
-        <v>14.832000000000001</v>
-      </c>
-      <c r="K13" s="15">
-        <v>20.683</v>
-      </c>
-      <c r="L13" s="16">
-        <v>4.07E-2</v>
-      </c>
-      <c r="M13" s="14">
-        <v>1.218</v>
-      </c>
-      <c r="N13" s="14">
-        <v>336262</v>
-      </c>
-      <c r="O13" s="14">
-        <v>0.90700000000000003</v>
-      </c>
-      <c r="P13" s="14">
-        <v>0.187</v>
-      </c>
-      <c r="Q13" s="14">
-        <v>336377</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="14">
-        <v>158</v>
-      </c>
-      <c r="C14" s="14">
-        <v>128</v>
-      </c>
-      <c r="D14" s="15">
-        <v>0.48499999999999999</v>
-      </c>
-      <c r="E14" s="14">
-        <v>1</v>
-      </c>
-      <c r="F14" s="15">
-        <v>17.68</v>
-      </c>
-      <c r="G14" s="16">
-        <v>1.24E-2</v>
-      </c>
-      <c r="H14" s="14">
-        <v>1.641</v>
-      </c>
-      <c r="I14" s="14">
-        <v>1.3100000000000001E-2</v>
-      </c>
-      <c r="J14" s="15">
-        <v>15.409000000000001</v>
-      </c>
-      <c r="K14" s="15">
-        <v>20</v>
-      </c>
-      <c r="L14" s="16">
-        <v>3.0999999999999999E-3</v>
-      </c>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="14"/>
-    </row>
-    <row r="15" spans="1:17" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="14">
-        <v>178</v>
-      </c>
-      <c r="C15" s="14">
-        <v>83</v>
-      </c>
-      <c r="D15" s="15">
-        <v>5.0999999999999997E-2</v>
-      </c>
-      <c r="E15" s="14">
-        <v>1</v>
-      </c>
-      <c r="F15" s="15">
-        <v>18</v>
-      </c>
-      <c r="G15" s="16">
-        <v>1.2200000000000001E-2</v>
-      </c>
-      <c r="H15" s="14">
-        <v>1.1919999999999999</v>
-      </c>
-      <c r="I15" s="14">
-        <v>1.2200000000000001E-2</v>
-      </c>
-      <c r="J15" s="15">
-        <v>14.478999999999999</v>
-      </c>
-      <c r="K15" s="15">
-        <v>19.963000000000001</v>
-      </c>
-      <c r="L15" s="16">
-        <v>2.5999999999999999E-3</v>
-      </c>
-      <c r="M15" s="14">
-        <v>0.66</v>
-      </c>
-      <c r="N15" s="14">
-        <v>22241</v>
-      </c>
-      <c r="O15" s="14">
-        <v>0.38800000000000001</v>
-      </c>
-      <c r="P15" s="14">
-        <v>0.75600000000000001</v>
-      </c>
-      <c r="Q15" s="14">
-        <v>22358</v>
       </c>
     </row>
     <row r="16" spans="1:17" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B16" s="14">
-        <v>106</v>
-      </c>
-      <c r="C16" s="14">
-        <v>150</v>
-      </c>
+        <v>2638</v>
+      </c>
+      <c r="C16" s="14"/>
       <c r="D16" s="15">
-        <v>0.19</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="E16" s="14">
-        <v>5.73</v>
+        <v>1</v>
       </c>
       <c r="F16" s="15">
-        <v>15.792</v>
+        <v>17.033000000000001</v>
       </c>
       <c r="G16" s="16">
-        <v>1.23E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="H16" s="14">
-        <v>0.55400000000000005</v>
+        <v>0.76400000000000001</v>
       </c>
       <c r="I16" s="14">
-        <v>1.1599999999999999E-2</v>
+        <v>4.9700000000000001E-2</v>
       </c>
       <c r="J16" s="15">
-        <v>14.757999999999999</v>
+        <v>14.832000000000001</v>
       </c>
       <c r="K16" s="15">
-        <v>18.475999999999999</v>
+        <v>20.683</v>
       </c>
       <c r="L16" s="16">
-        <v>2E-3</v>
+        <v>4.07E-2</v>
       </c>
       <c r="M16" s="14">
-        <v>8.9300000000000004E-2</v>
+        <v>1.218</v>
       </c>
       <c r="N16" s="14">
-        <v>21064</v>
+        <v>336262</v>
       </c>
       <c r="O16" s="14">
-        <v>5.6599999999999998E-2</v>
+        <v>0.90700000000000003</v>
       </c>
       <c r="P16" s="14">
-        <v>0.11</v>
+        <v>0.187</v>
       </c>
       <c r="Q16" s="14">
-        <v>21200</v>
+        <v>336377</v>
       </c>
     </row>
     <row r="17" spans="1:17" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B17" s="14">
-        <v>54</v>
+        <v>158</v>
       </c>
       <c r="C17" s="14">
-        <v>216</v>
+        <v>128</v>
       </c>
       <c r="D17" s="15">
-        <v>0.51</v>
+        <v>0.48499999999999999</v>
       </c>
       <c r="E17" s="14">
-        <v>4.68</v>
+        <v>1</v>
       </c>
       <c r="F17" s="15">
-        <v>16.425999999999998</v>
+        <v>17.68</v>
       </c>
       <c r="G17" s="16">
-        <v>1.0999999999999999E-2</v>
+        <v>1.24E-2</v>
       </c>
       <c r="H17" s="14">
-        <v>0.57299999999999995</v>
+        <v>1.641</v>
       </c>
       <c r="I17" s="14">
-        <v>1.0699999999999999E-2</v>
+        <v>1.3100000000000001E-2</v>
       </c>
       <c r="J17" s="15">
-        <v>14.808999999999999</v>
+        <v>15.409000000000001</v>
       </c>
       <c r="K17" s="15">
-        <v>18.559999999999999</v>
+        <v>20</v>
       </c>
       <c r="L17" s="16">
-        <v>1.2999999999999999E-3</v>
-      </c>
-      <c r="M17" s="14">
-        <v>0.16200000000000001</v>
-      </c>
-      <c r="N17" s="14">
-        <v>10885</v>
-      </c>
-      <c r="O17" s="14">
-        <v>9.2399999999999996E-2</v>
-      </c>
-      <c r="P17" s="14">
-        <v>0.16600000000000001</v>
-      </c>
-      <c r="Q17" s="14">
-        <v>10942</v>
-      </c>
+        <v>3.0999999999999999E-3</v>
+      </c>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14"/>
+      <c r="P17" s="14"/>
+      <c r="Q17" s="14"/>
     </row>
     <row r="18" spans="1:17" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B18" s="14">
-        <v>46</v>
+        <v>178</v>
       </c>
       <c r="C18" s="14">
-        <v>204</v>
+        <v>83</v>
       </c>
       <c r="D18" s="15">
-        <v>0.9</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="E18" s="14">
-        <v>8.01</v>
+        <v>1</v>
       </c>
       <c r="F18" s="15">
-        <v>16.716000000000001</v>
+        <v>18</v>
       </c>
       <c r="G18" s="16">
-        <v>1.0699999999999999E-2</v>
+        <v>1.2200000000000001E-2</v>
       </c>
       <c r="H18" s="14">
-        <v>0.58499999999999996</v>
+        <v>1.1919999999999999</v>
       </c>
       <c r="I18" s="14">
-        <v>1.0500000000000001E-2</v>
+        <v>1.2200000000000001E-2</v>
       </c>
       <c r="J18" s="15">
-        <v>14.821</v>
+        <v>14.478999999999999</v>
       </c>
       <c r="K18" s="15">
-        <v>18.61</v>
+        <v>19.963000000000001</v>
       </c>
       <c r="L18" s="16">
-        <v>2E-3</v>
+        <v>2.5999999999999999E-3</v>
       </c>
       <c r="M18" s="14">
-        <v>0.128</v>
+        <v>0.66</v>
       </c>
       <c r="N18" s="14">
-        <v>7915</v>
+        <v>22241</v>
       </c>
       <c r="O18" s="14">
-        <v>7.6499999999999999E-2</v>
+        <v>0.38800000000000001</v>
       </c>
       <c r="P18" s="14">
-        <v>0.14299999999999999</v>
+        <v>0.75600000000000001</v>
       </c>
       <c r="Q18" s="14">
-        <v>8046</v>
+        <v>22358</v>
       </c>
     </row>
     <row r="19" spans="1:17" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="14">
+        <v>106</v>
+      </c>
+      <c r="C19" s="14">
+        <v>150</v>
+      </c>
+      <c r="D19" s="15">
+        <v>0.19</v>
+      </c>
+      <c r="E19" s="14">
+        <v>5.73</v>
+      </c>
+      <c r="F19" s="15">
+        <v>15.792</v>
+      </c>
+      <c r="G19" s="16">
+        <v>1.23E-2</v>
+      </c>
+      <c r="H19" s="14">
+        <v>0.55400000000000005</v>
+      </c>
+      <c r="I19" s="14">
+        <v>1.1599999999999999E-2</v>
+      </c>
+      <c r="J19" s="15">
+        <v>14.757999999999999</v>
+      </c>
+      <c r="K19" s="15">
+        <v>18.475999999999999</v>
+      </c>
+      <c r="L19" s="16">
+        <v>2E-3</v>
+      </c>
+      <c r="M19" s="14">
+        <v>8.9300000000000004E-2</v>
+      </c>
+      <c r="N19" s="14">
+        <v>21064</v>
+      </c>
+      <c r="O19" s="14">
+        <v>5.6599999999999998E-2</v>
+      </c>
+      <c r="P19" s="14">
+        <v>0.11</v>
+      </c>
+      <c r="Q19" s="14">
+        <v>21200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="14">
+        <v>54</v>
+      </c>
+      <c r="C20" s="14">
+        <v>216</v>
+      </c>
+      <c r="D20" s="15">
+        <v>0.51</v>
+      </c>
+      <c r="E20" s="14">
+        <v>4.68</v>
+      </c>
+      <c r="F20" s="15">
+        <v>16.425999999999998</v>
+      </c>
+      <c r="G20" s="16">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="H20" s="14">
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="I20" s="14">
+        <v>1.0699999999999999E-2</v>
+      </c>
+      <c r="J20" s="15">
+        <v>14.808999999999999</v>
+      </c>
+      <c r="K20" s="15">
+        <v>18.559999999999999</v>
+      </c>
+      <c r="L20" s="16">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="M20" s="14">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="N20" s="14">
+        <v>10885</v>
+      </c>
+      <c r="O20" s="14">
+        <v>9.2399999999999996E-2</v>
+      </c>
+      <c r="P20" s="14">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="Q20" s="14">
+        <v>10942</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="14">
+        <v>46</v>
+      </c>
+      <c r="C21" s="14">
+        <v>204</v>
+      </c>
+      <c r="D21" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="E21" s="14">
+        <v>8.01</v>
+      </c>
+      <c r="F21" s="15">
+        <v>16.716000000000001</v>
+      </c>
+      <c r="G21" s="16">
+        <v>1.0699999999999999E-2</v>
+      </c>
+      <c r="H21" s="14">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="I21" s="14">
+        <v>1.0500000000000001E-2</v>
+      </c>
+      <c r="J21" s="15">
+        <v>14.821</v>
+      </c>
+      <c r="K21" s="15">
+        <v>18.61</v>
+      </c>
+      <c r="L21" s="16">
+        <v>2E-3</v>
+      </c>
+      <c r="M21" s="14">
+        <v>0.128</v>
+      </c>
+      <c r="N21" s="14">
+        <v>7915</v>
+      </c>
+      <c r="O21" s="14">
+        <v>7.6499999999999999E-2</v>
+      </c>
+      <c r="P21" s="14">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="Q21" s="14">
+        <v>8046</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="14">
+      <c r="B22" s="14">
         <v>46</v>
       </c>
-      <c r="C19" s="14">
+      <c r="C22" s="14">
         <v>410</v>
       </c>
-      <c r="D19" s="15">
+      <c r="D22" s="15">
         <v>16.2</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E22" s="14">
         <v>11.34</v>
       </c>
-      <c r="F19" s="15">
+      <c r="F22" s="15">
         <v>16.265000000000001</v>
       </c>
-      <c r="G19" s="16">
+      <c r="G22" s="16">
         <v>1.06E-2</v>
       </c>
-      <c r="H19" s="14">
+      <c r="H22" s="14">
         <v>14.146000000000001</v>
       </c>
-      <c r="I19" s="14">
+      <c r="I22" s="14">
         <v>1.04E-2</v>
       </c>
-      <c r="J19" s="15">
+      <c r="J22" s="15">
         <v>14.146000000000001</v>
       </c>
-      <c r="K19" s="15">
+      <c r="K22" s="15">
         <v>18.8</v>
       </c>
-      <c r="L19" s="16">
+      <c r="L22" s="16">
         <v>1.5E-3</v>
       </c>
-      <c r="M19" s="14">
+      <c r="M22" s="14">
         <v>0.63300000000000001</v>
       </c>
-      <c r="N19" s="14">
+      <c r="N22" s="14">
         <v>6668</v>
       </c>
-      <c r="O19" s="14">
+      <c r="O22" s="14">
         <v>0.33100000000000002</v>
       </c>
-      <c r="P19" s="14">
+      <c r="P22" s="14">
         <v>0.64700000000000002</v>
       </c>
-      <c r="Q19" s="14">
+      <c r="Q22" s="14">
         <v>6749</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="O11:Q11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="O14:Q14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D107C97-A11C-3242-B295-1DA8D8BA921C}">
+  <dimension ref="A2:Q18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="43.5" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="4"/>
+    <col min="6" max="6" width="10.83203125" style="4"/>
+    <col min="7" max="7" width="10.83203125" style="6"/>
+    <col min="10" max="11" width="10.83203125" style="4"/>
+    <col min="12" max="12" width="10.83203125" style="6"/>
+    <col min="16" max="16" width="11.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+    </row>
+    <row r="14" spans="1:17" s="1" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="8"/>
+      <c r="H14" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+    </row>
+    <row r="15" spans="1:17" s="3" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K15" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="L15" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="M15" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N15" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="O15" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="P15" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q15" s="12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="14">
+        <v>2624</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="15">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E16" s="14">
+        <v>1</v>
+      </c>
+      <c r="F16" s="15">
+        <v>13.01</v>
+      </c>
+      <c r="G16" s="16">
+        <v>5.04E-2</v>
+      </c>
+      <c r="H16" s="14">
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="I16" s="14">
+        <v>5.0299999999999997E-2</v>
+      </c>
+      <c r="J16" s="15">
+        <v>18.571999999999999</v>
+      </c>
+      <c r="K16" s="15">
+        <v>18.646999999999998</v>
+      </c>
+      <c r="L16" s="16">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="M16" s="14">
+        <v>0.93400000000000005</v>
+      </c>
+      <c r="N16" s="14">
+        <v>335084</v>
+      </c>
+      <c r="O16" s="14">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="P16" s="14">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="Q16" s="14">
+        <v>398099</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="14">
+        <v>168</v>
+      </c>
+      <c r="C17" s="14">
+        <v>63</v>
+      </c>
+      <c r="D17" s="15">
+        <v>0.308</v>
+      </c>
+      <c r="E17" s="14">
+        <v>1</v>
+      </c>
+      <c r="F17" s="15">
+        <v>17.242000000000001</v>
+      </c>
+      <c r="G17" s="16">
+        <v>1.3100000000000001E-2</v>
+      </c>
+      <c r="H17" s="14">
+        <v>1.431</v>
+      </c>
+      <c r="I17" s="14">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="J17" s="15">
+        <v>14.965999999999999</v>
+      </c>
+      <c r="K17" s="15">
+        <v>21.323</v>
+      </c>
+      <c r="L17" s="16">
+        <v>2.8E-3</v>
+      </c>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14">
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="P17" s="14">
+        <v>0.64300000000000002</v>
+      </c>
+      <c r="Q17" s="14">
+        <v>20920</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
+      <c r="P18" s="14"/>
+      <c r="Q18" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="O14:Q14"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
use OPT_PARAM('cell_offload_processing' 'false') to disable physical read from cell server
</commit_message>
<xml_diff>
--- a/OracleBenchmarks.xlsx
+++ b/OracleBenchmarks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pramm/Documents/Projekte/rammpeter.github/oracle_benchmarks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C000E3-D03A-4245-B6BE-D36AF19FF5D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96D73BC-448B-DB47-9A18-C9150C5FF9F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3160" yWindow="2260" windowWidth="28240" windowHeight="17240" activeTab="2" xr2:uid="{94BF2A6F-DF63-3D44-AC4F-74C7E5880432}"/>
   </bookViews>
@@ -3114,7 +3114,7 @@
   <dimension ref="A2:Q18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3323,7 +3323,7 @@
         <v>168</v>
       </c>
       <c r="C17" s="14">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D17" s="15">
         <v>0.308</v>
@@ -3344,46 +3344,82 @@
         <v>0.13100000000000001</v>
       </c>
       <c r="J17" s="15">
-        <v>14.965999999999999</v>
+        <v>13.744</v>
       </c>
       <c r="K17" s="15">
-        <v>21.323</v>
+        <v>18.977</v>
       </c>
       <c r="L17" s="16">
-        <v>2.8E-3</v>
-      </c>
-      <c r="M17" s="14"/>
-      <c r="N17" s="14"/>
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="M17" s="14">
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="N17" s="14">
+        <v>20812</v>
+      </c>
       <c r="O17" s="14">
-        <v>0.33600000000000002</v>
+        <v>0.34399999999999997</v>
       </c>
       <c r="P17" s="14">
-        <v>0.64300000000000002</v>
+        <v>0.63300000000000001</v>
       </c>
       <c r="Q17" s="14">
-        <v>20920</v>
+        <v>21137</v>
       </c>
     </row>
     <row r="18" spans="1:17" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="16"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="14"/>
-      <c r="O18" s="14"/>
-      <c r="P18" s="14"/>
-      <c r="Q18" s="14"/>
+      <c r="B18" s="14">
+        <v>168</v>
+      </c>
+      <c r="C18" s="14">
+        <v>60</v>
+      </c>
+      <c r="D18" s="15">
+        <v>0.29699999999999999</v>
+      </c>
+      <c r="E18" s="14">
+        <v>1</v>
+      </c>
+      <c r="F18" s="15">
+        <v>16.956</v>
+      </c>
+      <c r="G18" s="16">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="H18" s="14">
+        <v>1.4219999999999999</v>
+      </c>
+      <c r="I18" s="14">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="J18" s="15">
+        <v>14.182</v>
+      </c>
+      <c r="K18" s="15">
+        <v>19.933</v>
+      </c>
+      <c r="L18" s="16">
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="M18" s="14">
+        <v>0.626</v>
+      </c>
+      <c r="N18" s="14">
+        <v>20812</v>
+      </c>
+      <c r="O18" s="14">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="P18" s="14">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="Q18" s="14">
+        <v>21115</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>